<commit_message>
Added docs and examples. Improved architecture
</commit_message>
<xml_diff>
--- a/docs/theory.xlsx
+++ b/docs/theory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.kuprin\source\repos\Dithering\Dithering\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE10FC0-AB67-46E6-B7DD-B82B874561D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1955C6-10D0-49AE-86BA-4B97070BB13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>количество потоков</t>
   </si>
@@ -94,25 +94,22 @@
     <t>VGA 256 colors (Neon)</t>
   </si>
   <si>
-    <t>картинка 1 (кот) способ 2 без использования ускоряющих структур</t>
+    <t>Black and white</t>
   </si>
   <si>
-    <t>картинка 1 (кот) способ 2 с использованием ускоряющих структур</t>
+    <t>Four-bit grayscale</t>
   </si>
   <si>
-    <t>0 Black and white</t>
+    <t>EGA 16 colors</t>
   </si>
   <si>
-    <t>2 Two-bit grayscale</t>
+    <t>VGA 256 colors</t>
   </si>
   <si>
-    <t>3Four-bit grayscale</t>
+    <t>картинка кот</t>
   </si>
   <si>
-    <t>15 EGA 16 colors</t>
-  </si>
-  <si>
-    <t>16 VGA 256 colors</t>
+    <t>Black , gray and white</t>
   </si>
 </sst>
 </file>
@@ -206,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,6 +217,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,22 +246,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,6 +275,2075 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Black and white</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$42:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>198.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3242-4FB5-BD0F-C2692563167A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Black , gray and white</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$43:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>111.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3242-4FB5-BD0F-C2692563167A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Four-bit grayscale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>262.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>166.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>154.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3242-4FB5-BD0F-C2692563167A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EGA 16 colors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$45:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>238.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>157.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.19999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3242-4FB5-BD0F-C2692563167A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="136743328"/>
+        <c:axId val="136743744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="136743328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="136743744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="136743744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="136743328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VGA 256 colors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$46:$I$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>477.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>390.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>296.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>342.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BE6A-4BF1-8300-42040C51272E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="148847792"/>
+        <c:axId val="148852784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="148847792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148852784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="148852784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="148847792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66EDBB2B-36EF-439C-9420-8D0C90DACC74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51339573-D290-4002-B9DB-750293887DDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,10 +2643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" activeCellId="1" sqref="A41:I41 A46:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,714 +3565,482 @@
       <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="8">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="12">
         <v>290</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10">
         <v>227</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10">
         <v>227</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <v>210</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10">
         <v>362</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10">
         <v>362</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10">
         <v>362</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10">
         <v>362</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10">
         <v>362</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10">
         <v>362</v>
       </c>
-      <c r="F30" s="6"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10">
         <v>362</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10">
         <v>310</v>
       </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10">
         <v>320</v>
       </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10">
         <v>290</v>
       </c>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10">
         <v>290</v>
       </c>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10">
         <v>150</v>
       </c>
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10">
         <v>90</v>
       </c>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="39" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="F37" s="10"/>
+    </row>
+    <row r="39" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+    </row>
+    <row r="41" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="5">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>4</v>
+      </c>
+      <c r="H41" s="5">
+        <v>6</v>
+      </c>
+      <c r="I41" s="5">
+        <v>8</v>
+      </c>
+      <c r="J41" s="7"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39"/>
-    </row>
-    <row r="40" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="5">
-        <v>1</v>
-      </c>
-      <c r="F40" s="5">
-        <v>2</v>
-      </c>
-      <c r="G40" s="5">
-        <v>3</v>
-      </c>
-      <c r="H40" s="5">
-        <v>4</v>
-      </c>
-      <c r="I40" s="5">
-        <v>5</v>
-      </c>
-      <c r="J40" s="5">
-        <v>6</v>
-      </c>
-      <c r="K40" s="5">
-        <v>7</v>
-      </c>
-      <c r="L40" s="5">
-        <v>8</v>
-      </c>
-      <c r="M40"/>
-    </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="5">
+        <v>198.2</v>
+      </c>
+      <c r="F42" s="5">
+        <v>109.8</v>
+      </c>
+      <c r="G42" s="5">
+        <v>87.8</v>
+      </c>
+      <c r="H42" s="5">
+        <v>69.2</v>
+      </c>
+      <c r="I42" s="5">
+        <v>121.6</v>
+      </c>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+    </row>
+    <row r="43" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="5">
+        <v>189</v>
+      </c>
+      <c r="F43" s="5">
+        <v>111.6</v>
+      </c>
+      <c r="G43" s="5">
+        <v>89.2</v>
+      </c>
+      <c r="H43" s="5">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="I43" s="5">
+        <v>120.4</v>
+      </c>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+    </row>
+    <row r="44" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="5">
+        <v>262.39999999999998</v>
+      </c>
+      <c r="F44" s="5">
+        <v>166.6</v>
+      </c>
+      <c r="G44" s="5">
+        <v>121.2</v>
+      </c>
+      <c r="H44" s="5">
+        <v>92.6</v>
+      </c>
+      <c r="I44" s="5">
+        <v>154.6</v>
+      </c>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+    </row>
+    <row r="45" spans="1:16" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="5">
-        <v>224</v>
-      </c>
-      <c r="F41" s="5">
-        <v>182</v>
-      </c>
-      <c r="G41" s="5">
-        <v>164</v>
-      </c>
-      <c r="H41" s="5">
-        <v>179</v>
-      </c>
-      <c r="I41" s="5">
-        <v>195</v>
-      </c>
-      <c r="J41" s="5">
-        <v>189</v>
-      </c>
-      <c r="K41" s="5">
-        <v>200</v>
-      </c>
-      <c r="L41" s="5">
-        <v>207</v>
-      </c>
-      <c r="M41"/>
-    </row>
-    <row r="42" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="5">
+        <v>238.6</v>
+      </c>
+      <c r="F45" s="5">
+        <v>157.6</v>
+      </c>
+      <c r="G45" s="5">
+        <v>108.4</v>
+      </c>
+      <c r="H45" s="5">
+        <v>83.4</v>
+      </c>
+      <c r="I45" s="5">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+    </row>
+    <row r="46" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="5">
-        <v>228</v>
-      </c>
-      <c r="F42" s="5">
-        <v>174</v>
-      </c>
-      <c r="G42" s="5">
-        <v>161</v>
-      </c>
-      <c r="H42" s="5">
-        <v>177</v>
-      </c>
-      <c r="I42" s="5">
-        <v>185</v>
-      </c>
-      <c r="J42" s="5">
-        <v>205</v>
-      </c>
-      <c r="K42" s="5">
-        <v>202</v>
-      </c>
-      <c r="L42" s="5">
-        <v>224</v>
-      </c>
-      <c r="M42"/>
-    </row>
-    <row r="43" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="5">
-        <v>283</v>
-      </c>
-      <c r="F43" s="5">
-        <v>202</v>
-      </c>
-      <c r="G43" s="5">
-        <v>189</v>
-      </c>
-      <c r="H43" s="5">
-        <v>196</v>
-      </c>
-      <c r="I43" s="5">
-        <v>203</v>
-      </c>
-      <c r="J43" s="5">
-        <v>205</v>
-      </c>
-      <c r="K43" s="5">
-        <v>238</v>
-      </c>
-      <c r="L43" s="5">
-        <v>254</v>
-      </c>
-      <c r="M43"/>
-    </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="5">
-        <v>286</v>
-      </c>
-      <c r="F44" s="5">
-        <v>197</v>
-      </c>
-      <c r="G44" s="5">
-        <v>197</v>
-      </c>
-      <c r="H44" s="5">
-        <v>202</v>
-      </c>
-      <c r="I44" s="5">
-        <v>204</v>
-      </c>
-      <c r="J44" s="5">
-        <v>225</v>
-      </c>
-      <c r="K44" s="5">
-        <v>237</v>
-      </c>
-      <c r="L44" s="5">
-        <v>240</v>
-      </c>
-      <c r="M44"/>
-    </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="5">
-        <v>1118</v>
-      </c>
-      <c r="F45" s="5">
-        <v>675</v>
-      </c>
-      <c r="G45" s="5">
-        <v>597</v>
-      </c>
-      <c r="H45" s="5">
-        <v>596</v>
-      </c>
-      <c r="I45" s="5">
-        <v>547</v>
-      </c>
-      <c r="J45" s="5">
-        <v>513</v>
-      </c>
-      <c r="K45" s="5">
-        <v>493</v>
-      </c>
-      <c r="L45" s="5">
-        <v>509</v>
-      </c>
-      <c r="M45"/>
-    </row>
-    <row r="46" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="5">
+        <v>738</v>
+      </c>
+      <c r="F46" s="5">
+        <v>477.8</v>
+      </c>
+      <c r="G46" s="5">
+        <v>390.4</v>
+      </c>
+      <c r="H46" s="5">
+        <v>296.2</v>
+      </c>
+      <c r="I46" s="5">
+        <v>342.8</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
       <c r="M46"/>
     </row>
-    <row r="47" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
+    <row r="47" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="5">
-        <v>1</v>
-      </c>
-      <c r="F48" s="5">
-        <v>2</v>
-      </c>
-      <c r="G48" s="5">
-        <v>3</v>
-      </c>
-      <c r="H48" s="5">
-        <v>4</v>
-      </c>
-      <c r="I48" s="5">
-        <v>5</v>
-      </c>
-      <c r="J48" s="5">
-        <v>6</v>
-      </c>
-      <c r="K48" s="5">
-        <v>7</v>
-      </c>
-      <c r="L48" s="5">
-        <v>8</v>
-      </c>
+    <row r="48" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
       <c r="M48"/>
     </row>
-    <row r="49" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="5">
-        <v>238</v>
-      </c>
-      <c r="F49" s="5">
-        <v>187</v>
-      </c>
-      <c r="G49" s="5">
-        <v>169</v>
-      </c>
-      <c r="H49" s="5">
-        <v>192</v>
-      </c>
-      <c r="I49" s="5">
-        <v>189</v>
-      </c>
-      <c r="J49" s="5">
-        <v>198</v>
-      </c>
-      <c r="K49" s="5">
-        <v>202</v>
-      </c>
-      <c r="L49" s="5">
-        <v>219</v>
-      </c>
+    <row r="49" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
       <c r="M49"/>
     </row>
-    <row r="50" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5">
-        <v>237</v>
-      </c>
-      <c r="F50" s="5">
-        <v>177</v>
-      </c>
-      <c r="G50" s="5">
-        <v>172</v>
-      </c>
-      <c r="H50" s="5">
-        <v>178</v>
-      </c>
-      <c r="I50" s="5">
-        <v>185</v>
-      </c>
-      <c r="J50" s="5">
-        <v>198</v>
-      </c>
-      <c r="K50" s="5">
-        <v>213</v>
-      </c>
-      <c r="L50" s="5">
-        <v>222</v>
-      </c>
-      <c r="M50"/>
-    </row>
-    <row r="51" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="5">
-        <v>309</v>
-      </c>
-      <c r="F51" s="5">
-        <v>210</v>
-      </c>
-      <c r="G51" s="5">
-        <v>234</v>
-      </c>
-      <c r="H51" s="5">
-        <v>202</v>
-      </c>
-      <c r="I51" s="5">
-        <v>216</v>
-      </c>
-      <c r="J51" s="5">
-        <v>220</v>
-      </c>
-      <c r="K51" s="5">
-        <v>232</v>
-      </c>
-      <c r="L51" s="5">
-        <v>251</v>
-      </c>
-      <c r="M51"/>
-    </row>
-    <row r="52" spans="1:13" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="5">
-        <v>284</v>
-      </c>
-      <c r="F52" s="5">
-        <v>206</v>
-      </c>
-      <c r="G52" s="5">
-        <v>191</v>
-      </c>
-      <c r="H52" s="5">
-        <v>199</v>
-      </c>
-      <c r="I52" s="5">
-        <v>200</v>
-      </c>
-      <c r="J52" s="5">
-        <v>218</v>
-      </c>
-      <c r="K52" s="5">
-        <v>224</v>
-      </c>
-      <c r="L52" s="5">
-        <v>253</v>
-      </c>
-      <c r="M52"/>
-    </row>
-    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="5">
-        <v>785</v>
-      </c>
-      <c r="F53" s="5">
-        <v>532</v>
-      </c>
-      <c r="G53" s="5">
-        <v>458</v>
-      </c>
-      <c r="H53" s="5">
-        <v>454</v>
-      </c>
-      <c r="I53" s="5">
-        <v>435</v>
-      </c>
-      <c r="J53" s="5">
-        <v>419</v>
-      </c>
-      <c r="K53" s="5">
-        <v>415</v>
-      </c>
-      <c r="L53" s="5">
-        <v>420</v>
-      </c>
-      <c r="M53"/>
-    </row>
-    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-    </row>
-    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="K55"/>
-      <c r="L55"/>
-      <c r="M55"/>
-    </row>
-    <row r="56" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56"/>
-      <c r="L56"/>
-      <c r="M56"/>
-    </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="A53:D53"/>
+  <mergeCells count="43">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A46:D46"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
@@ -2212,7 +4055,7 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A20:D20"/>
@@ -2228,27 +4071,20 @@
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A40:I40"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>